<commit_message>
Add RecommendPath & MsgDel
</commit_message>
<xml_diff>
--- a/GeumEServer/Upload/PlaceList.xlsx
+++ b/GeumEServer/Upload/PlaceList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Newcl\Desktop\GeumEServer\GeumEServer\Upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F0D954-4091-45B5-9B20-ABA76C92E370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54702003-961D-4EA7-84E8-9A35F64775A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F3874724-14C7-4AA2-B629-E79FF8C39947}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F3874724-14C7-4AA2-B629-E79FF8C39947}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="113">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -598,6 +598,577 @@
   </si>
   <si>
     <t>간식</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>효창공원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>서울</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>용산구</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>효창원로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> 177-18 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>효창공원</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>서울</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>용산구</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>청파동</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>가</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>원효로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>97</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>길</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 50</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>돌모루어린이공원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 용산구 문배동 45</t>
+  </si>
+  <si>
+    <t>해님공원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>서울</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>용산구</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>문배동</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 24-1</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>문배어린이공원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>서울</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>용산구</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>청파로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 139-25</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>신계역사공원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>솔밭어린이공원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>서울</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>용산구</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>서빙고로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 137</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>용산공원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>서울</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>용산구</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>이촌로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>72</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>길</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 62</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이촌 한강공원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 용산구 녹사평대로40다길 33</t>
+  </si>
+  <si>
+    <t>이태원부군당역사공원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>서울</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>용산구</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>한강로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>가</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 30-3</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -605,7 +1176,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -660,6 +1231,26 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="3"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1014,13 +1605,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2363CFA0-5CD6-4ABE-B435-F0B915AF01FB}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="2" max="2" width="27.5" customWidth="1"/>
     <col min="3" max="3" width="12.625" customWidth="1"/>
@@ -1029,7 +1620,7 @@
     <col min="7" max="7" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1052,7 +1643,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1075,7 +1666,7 @@
         <v>126.970077</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1098,7 +1689,7 @@
         <v>126.973236</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1121,7 +1712,7 @@
         <v>126.96605599999999</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1144,7 +1735,7 @@
         <v>126.972760951596</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1167,7 +1758,7 @@
         <v>126.97626108963</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1190,7 +1781,7 @@
         <v>126.978669278304</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1213,7 +1804,7 @@
         <v>126.985207448903</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1236,7 +1827,7 @@
         <v>126.98424868980401</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1259,7 +1850,7 @@
         <v>126.987533125974</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1282,7 +1873,7 @@
         <v>126.987558587016</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1305,7 +1896,7 @@
         <v>126.99275829141401</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1328,7 +1919,7 @@
         <v>126.99579643557701</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1351,7 +1942,7 @@
         <v>126.99105839431201</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1374,7 +1965,7 @@
         <v>126.98802351050701</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1397,7 +1988,7 @@
         <v>127.001518978551</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1420,7 +2011,7 @@
         <v>127.004486188801</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1443,7 +2034,7 @@
         <v>127.004486188801</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1466,7 +2057,7 @@
         <v>127.011628465237</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1489,7 +2080,7 @@
         <v>127.011628465237</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1512,7 +2103,7 @@
         <v>127.00174235929499</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1535,7 +2126,7 @@
         <v>126.990244491269</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1558,7 +2149,7 @@
         <v>126.98954288055801</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1581,7 +2172,7 @@
         <v>126.995036120165</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1604,7 +2195,7 @@
         <v>127.00001696952999</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1627,7 +2218,7 @@
         <v>126.968521111675</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1650,7 +2241,7 @@
         <v>126.970954940328</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1673,7 +2264,7 @@
         <v>126.962994017699</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1696,7 +2287,7 @@
         <v>126.96787741083899</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1719,7 +2310,7 @@
         <v>126.962811673963</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1742,7 +2333,7 @@
         <v>126.95297361530901</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="17.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1765,7 +2356,7 @@
         <v>126.961842853863</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1788,7 +2379,7 @@
         <v>126.96338067526899</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1811,7 +2402,7 @@
         <v>126.961298392877</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1834,7 +2425,7 @@
         <v>126.961304054834</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1857,7 +2448,7 @@
         <v>126.963905696653</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1880,7 +2471,7 @@
         <v>126.965948079219</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1903,7 +2494,7 @@
         <v>126.95793966108801</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1925,9 +2516,236 @@
       <c r="G39" s="4">
         <v>126.968001013288</v>
       </c>
+    </row>
+    <row r="40" spans="1:7" ht="17.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>94</v>
+      </c>
+      <c r="C40" t="s">
+        <v>95</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F40" s="4">
+        <v>37.545110178521398</v>
+      </c>
+      <c r="G40" s="4">
+        <v>126.961068083736</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="17.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>98</v>
+      </c>
+      <c r="C41" t="s">
+        <v>95</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F41" s="4">
+        <v>37.542977022852902</v>
+      </c>
+      <c r="G41" s="4">
+        <v>126.96848647050101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>100</v>
+      </c>
+      <c r="C42" t="s">
+        <v>95</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F42" s="4">
+        <v>37.556600594892402</v>
+      </c>
+      <c r="G42" s="4">
+        <v>126.874403955506</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="17.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>102</v>
+      </c>
+      <c r="C43" t="s">
+        <v>95</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F43" s="4">
+        <v>37.536589282950601</v>
+      </c>
+      <c r="G43" s="4">
+        <v>126.969827096602</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="17.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>104</v>
+      </c>
+      <c r="C44" t="s">
+        <v>95</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F44" s="4">
+        <v>37.535043109164903</v>
+      </c>
+      <c r="G44" s="4">
+        <v>126.96628635890499</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="17.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>105</v>
+      </c>
+      <c r="C45" t="s">
+        <v>95</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F45" s="4">
+        <v>37.537392077101202</v>
+      </c>
+      <c r="G45" s="4">
+        <v>126.97360019432899</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="17.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>107</v>
+      </c>
+      <c r="C46" t="s">
+        <v>95</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F46" s="4">
+        <v>37.520121701194299</v>
+      </c>
+      <c r="G46" s="4">
+        <v>126.983707894516</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="17.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>109</v>
+      </c>
+      <c r="C47" t="s">
+        <v>95</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F47" s="4">
+        <v>37.517222421616303</v>
+      </c>
+      <c r="G47" s="4">
+        <v>126.97052490121401</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>111</v>
+      </c>
+      <c r="C48" t="s">
+        <v>95</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F48" s="4">
+        <v>37.5357637743232</v>
+      </c>
+      <c r="G48" s="4">
+        <v>126.98977464661201</v>
+      </c>
+    </row>
+    <row r="49" spans="6:7">
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+    </row>
+    <row r="50" spans="6:7">
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+    </row>
+    <row r="51" spans="6:7">
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+    </row>
+    <row r="52" spans="6:7">
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+    </row>
+    <row r="53" spans="6:7">
+      <c r="G53" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>